<commit_message>
Stats second lot twitter scrape.
</commit_message>
<xml_diff>
--- a/results/agg_results.xlsx
+++ b/results/agg_results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="183">
   <si>
     <t>Models</t>
   </si>
@@ -515,6 +515,69 @@
   <si>
     <t>I-
 character_assasination</t>
+  </si>
+  <si>
+    <t>बोका</t>
+  </si>
+  <si>
+    <t>तेरिमा</t>
+  </si>
+  <si>
+    <t>गुखाने</t>
+  </si>
+  <si>
+    <t>सुकुल गुन्डा</t>
+  </si>
+  <si>
+    <t>हरिलठक</t>
+  </si>
+  <si>
+    <t>बादरनी OR बादर</t>
+  </si>
+  <si>
+    <t>घिन लाग्दो</t>
+  </si>
+  <si>
+    <t>कालो मान्छे</t>
+  </si>
+  <si>
+    <t xml:space="preserve">पाखे OR पखिनी </t>
+  </si>
+  <si>
+    <t>पातकी</t>
+  </si>
+  <si>
+    <t>जाठी</t>
+  </si>
+  <si>
+    <t>माचिक्नि</t>
+  </si>
+  <si>
+    <t>बोक्सी</t>
+  </si>
+  <si>
+    <t>यौनकर्मी</t>
+  </si>
+  <si>
+    <t>डामाडोल</t>
+  </si>
+  <si>
+    <t>गोल्ड डीगर</t>
+  </si>
+  <si>
+    <t>बाह्र सत्ताइस</t>
+  </si>
+  <si>
+    <t>पोईमारा</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>scraped</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -525,7 +588,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,6 +686,19 @@
       <color theme="1" tint="0.34998626667073579"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -728,7 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -926,6 +1002,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2992,10 +3080,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:H20"/>
+  <dimension ref="C4:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24:M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3006,6 +3094,8 @@
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -3236,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:13" ht="21" x14ac:dyDescent="0.25">
       <c r="C17" s="46" t="s">
         <v>157</v>
       </c>
@@ -3256,7 +3346,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="18" spans="3:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" ht="21" x14ac:dyDescent="0.25">
       <c r="C18" s="46" t="s">
         <v>157</v>
       </c>
@@ -3276,7 +3366,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="19" spans="3:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13" ht="21" x14ac:dyDescent="0.25">
       <c r="C19" s="46" t="s">
         <v>157</v>
       </c>
@@ -3296,7 +3386,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="20" spans="3:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13" ht="21" x14ac:dyDescent="0.25">
       <c r="C20" s="46" t="s">
         <v>157</v>
       </c>
@@ -3314,6 +3404,167 @@
       </c>
       <c r="H20" s="51">
         <v>-100</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="L24" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="M24" s="72" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L25" s="70" t="s">
+        <v>162</v>
+      </c>
+      <c r="M25" s="71">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L26" s="70" t="s">
+        <v>163</v>
+      </c>
+      <c r="M26" s="71">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L27" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="M27" s="71">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L28" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="M28" s="71">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L29" s="70" t="s">
+        <v>166</v>
+      </c>
+      <c r="M29" s="71">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L30" s="70" t="s">
+        <v>167</v>
+      </c>
+      <c r="M30" s="71">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L31" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="M31" s="71">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L32" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="M32" s="71">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L33" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="M33" s="71">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L34" s="70" t="s">
+        <v>171</v>
+      </c>
+      <c r="M34" s="71">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L35" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="M35" s="71">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L36" s="70" t="s">
+        <v>173</v>
+      </c>
+      <c r="M36" s="71">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L37" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="M37" s="71">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L38" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="M38" s="71">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L39" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="M39" s="71">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L40" s="70" t="s">
+        <v>177</v>
+      </c>
+      <c r="M40" s="71">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L41" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="M41" s="71">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L42" s="70" t="s">
+        <v>179</v>
+      </c>
+      <c r="M42" s="71">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="12:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L43" s="73" t="s">
+        <v>182</v>
+      </c>
+      <c r="M43" s="73">
+        <f>SUM(M25:M42)</f>
+        <v>1107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>